<commit_message>
Added precision current measurement.
</commit_message>
<xml_diff>
--- a/doc/power consumption.xlsx
+++ b/doc/power consumption.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\o\CustomerProjects\Leoni\same54_sleep_adc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68F6183-74DD-4E6F-BD3B-E2C0EAB49E18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3EA4DD-65AF-48F3-A962-F6C86DAEE112}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="20865" windowHeight="5670" xr2:uid="{A4AD4609-0F22-4268-863C-ED41264E8E67}"/>
+    <workbookView xWindow="1890" yWindow="0" windowWidth="20865" windowHeight="5670" xr2:uid="{A4AD4609-0F22-4268-863C-ED41264E8E67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Time</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>µA avg</t>
+  </si>
+  <si>
+    <t>µA Keithley</t>
   </si>
 </sst>
 </file>
@@ -258,6 +261,160 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9DEF-4B36-A6A0-E4424843EB4E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>111.11111111111111</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>142.85714285714286</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>166.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>250.00000000000065</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>333.33333333333445</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>500.0000000000025</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1000.00000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>29.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>106.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>133.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>271</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7D8E-4AD5-A806-BC4163FDEFC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1009,16 +1166,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1343,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF28F5A8-7BD8-44D2-8B0E-69A059090D7C}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,7 +1513,7 @@
     <col min="4" max="4" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1369,8 +1526,11 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1383,8 +1543,11 @@
       <c r="D2" s="2">
         <v>32.6</v>
       </c>
+      <c r="E2">
+        <v>29.1</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1399,8 +1562,11 @@
       <c r="D3" s="2">
         <v>32.6</v>
       </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.1</v>
       </c>
@@ -1415,8 +1581,11 @@
       <c r="D4" s="2">
         <v>31.1</v>
       </c>
+      <c r="E4">
+        <v>35.9</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.05</v>
       </c>
@@ -1431,8 +1600,11 @@
       <c r="D5" s="2">
         <v>29.8</v>
       </c>
+      <c r="E5">
+        <v>43.1</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.02</v>
       </c>
@@ -1447,8 +1619,11 @@
       <c r="D6" s="2">
         <v>29.3</v>
       </c>
+      <c r="E6">
+        <v>66.599999999999994</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.01</v>
       </c>
@@ -1463,8 +1638,11 @@
       <c r="D7" s="2">
         <v>20.9</v>
       </c>
+      <c r="E7">
+        <v>94</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8.9999999999999993E-3</v>
       </c>
@@ -1479,8 +1657,11 @@
       <c r="D8" s="2">
         <v>17.8</v>
       </c>
+      <c r="E8">
+        <v>98</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -1495,8 +1676,11 @@
       <c r="D9" s="2">
         <v>17.7</v>
       </c>
+      <c r="E9">
+        <v>100.8</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -1511,8 +1695,11 @@
       <c r="D10" s="2">
         <v>19.100000000000001</v>
       </c>
+      <c r="E10">
+        <v>106.8</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -1527,8 +1714,11 @@
       <c r="D11" s="2">
         <v>40.4</v>
       </c>
+      <c r="E11">
+        <v>103</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1543,8 +1733,11 @@
       <c r="D12" s="2">
         <v>74.8</v>
       </c>
+      <c r="E12">
+        <v>106</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3.9999999999999897E-3</v>
       </c>
@@ -1559,8 +1752,11 @@
       <c r="D13" s="2">
         <v>119.3</v>
       </c>
+      <c r="E13">
+        <v>116</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2.9999999999999901E-3</v>
       </c>
@@ -1575,8 +1771,11 @@
       <c r="D14" s="2">
         <v>136</v>
       </c>
+      <c r="E14">
+        <v>133.5</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.9999999999999901E-3</v>
       </c>
@@ -1591,8 +1790,11 @@
       <c r="D15" s="2">
         <v>171</v>
       </c>
+      <c r="E15">
+        <v>166</v>
+      </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9.9999999999999005E-4</v>
       </c>
@@ -1606,6 +1808,9 @@
       </c>
       <c r="D16" s="2">
         <v>281.3</v>
+      </c>
+      <c r="E16">
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>